<commit_message>
Enroll and Sponsor ID changed in Excel sheet
</commit_message>
<xml_diff>
--- a/TestData/Enroll.xlsx
+++ b/TestData/Enroll.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="667"/>
@@ -257,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,7 +504,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>107594401</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>107804801</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>